<commit_message>
added table for video data
</commit_message>
<xml_diff>
--- a/Lab4/statistikk.xlsx
+++ b/Lab4/statistikk.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benja\Documents\Sensorer og instrumentering\SensorLab\Lab4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F5D5FAC-5A0D-4CF8-BD58-ACAF01A2E222}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{418DCE3F-739C-4D37-AEBE-A8D80AE3A2FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{47969C32-0EC6-4B6C-BB47-0B8C47DD7BD8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
   <si>
     <t>Sakte</t>
   </si>
@@ -56,7 +56,10 @@
     <t>STD</t>
   </si>
   <si>
-    <t>Reell verdi</t>
+    <t>Video</t>
+  </si>
+  <si>
+    <t>Radar [m/s]</t>
   </si>
 </sst>
 </file>
@@ -92,8 +95,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C1EC50E-1106-479F-8402-A9A0400F21D2}">
-  <dimension ref="A2:D10"/>
+  <dimension ref="A2:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B2" sqref="B2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -439,116 +445,178 @@
     <col min="1" max="1" width="11.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
+      <c r="E3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
         <v>0.74399999999999999</v>
       </c>
-      <c r="C3">
+      <c r="C4">
         <v>2.6850000000000001</v>
       </c>
-      <c r="D3">
+      <c r="D4">
         <v>-0.495</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4">
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B5">
         <v>0.95</v>
       </c>
-      <c r="C4">
+      <c r="C5">
         <v>2.3380000000000001</v>
       </c>
-      <c r="D4">
+      <c r="D5">
         <v>-0.36199999999999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5">
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <v>0.70899999999999996</v>
       </c>
-      <c r="C5">
+      <c r="C6">
         <v>2.1589999999999998</v>
       </c>
-      <c r="D5">
+      <c r="D6">
         <v>-0.82399999999999995</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7">
         <v>4</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <v>0.62</v>
       </c>
-      <c r="C6">
+      <c r="C7">
         <v>2.202</v>
       </c>
-      <c r="D6">
+      <c r="D7">
         <v>-0.78900000000000003</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>4</v>
       </c>
-      <c r="B7">
-        <f>AVERAGE(B3:B6)</f>
+      <c r="B8">
+        <f>AVERAGE(B4:B7)</f>
         <v>0.75575000000000003</v>
       </c>
-      <c r="C7">
-        <f t="shared" ref="C7:D7" si="0">AVERAGE(C3:C6)</f>
+      <c r="C8">
+        <f t="shared" ref="C8:D8" si="0">AVERAGE(C4:C7)</f>
         <v>2.3460000000000001</v>
       </c>
-      <c r="D7">
-        <f t="shared" si="0"/>
+      <c r="D8">
+        <f>AVERAGE(D4:D7)</f>
         <v>-0.61750000000000005</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="E8">
+        <f>AVERAGE(E4:E7)</f>
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <f t="shared" ref="F8:G8" si="1">AVERAGE(F4:F7)</f>
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <f>AVERAGE(G4:G7)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>5</v>
       </c>
-      <c r="B8">
-        <f>STDEV(B3:B6)</f>
+      <c r="B9">
+        <f>STDEV(B4:B7)</f>
         <v>0.13962419799829334</v>
       </c>
-      <c r="C8">
-        <f t="shared" ref="C8:D8" si="1">STDEV(C3:C6)</f>
+      <c r="C9">
+        <f t="shared" ref="C9:D9" si="2">STDEV(C4:C7)</f>
         <v>0.23853022170506341</v>
       </c>
-      <c r="D8">
-        <f t="shared" si="1"/>
+      <c r="D9">
+        <f>STDEV(D4:D7)</f>
         <v>0.22534492080660085</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>6</v>
+      <c r="E9">
+        <f>STDEV(E4:E7)</f>
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <f t="shared" ref="F9:G9" si="3">STDEV(F4:F7)</f>
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <f>STDEV(G4:G7)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:G2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>